<commit_message>
Finalised dialog, improved AdjustPointer
A canvas update is forced when ScrollChoiceBox is initialised so the pointer ends in the right place. The dialog is ready for final release.
Currently need one more fix for an issue with choice selection (can't betray darf until learning floral diplomacy from the bee, even though choice is there it's not selectabnle) and then ready for final release
</commit_message>
<xml_diff>
--- a/dialog.xlsx
+++ b/dialog.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\Unity Projects\TalkQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B8CB6A-D668-4F11-AAC0-73EC67962AC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C4DCB3-A9DD-4A1C-B186-A11FD5A870CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A16DE519-82AC-48F7-BFC5-13BDB3234C7E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28665" windowHeight="15600" activeTab="2" xr2:uid="{A16DE519-82AC-48F7-BFC5-13BDB3234C7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Darf" sheetId="2" r:id="rId2"/>
     <sheet name="Flowers" sheetId="4" r:id="rId3"/>
     <sheet name="Bee" sheetId="3" r:id="rId4"/>
-    <sheet name="Crinkle" sheetId="5" r:id="rId5"/>
-    <sheet name="Finkle" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="160">
   <si>
     <t>portrait</t>
   </si>
@@ -190,9 +188,6 @@
     <t>FlowerStrike</t>
   </si>
   <si>
-    <t>COUNTER</t>
-  </si>
-  <si>
     <t xml:space="preserve">So that's how it is. </t>
   </si>
   <si>
@@ -301,9 +296,6 @@
     <t>bzbz / bzbuzzbzbz bzbz buzz bz bzbuzzbz bzbuzz bzbuzzbzbz bzbuzzbzbz buzzbzbuzzbuzz / buzzbzbz buzzbuzzbuzz / buzzbz buzzbuzzbuzz buzz / bzbzbzbz bzbuzz bzbzbzbuzz bz / bzbzbzbuzz buzzbuzzbuzz buzzbzbuzzbz bzbuzz bzbuzzbzbz / buzzbzbuzzbz buzzbuzzbuzz bzbuzzbz buzzbzbz bzbzbz</t>
   </si>
   <si>
-    <t>28th</t>
-  </si>
-  <si>
     <t>bzbz bzbzbuzzbz / buzzbzbuzzbuzz buzzbuzzbuzz bzbzbuzz bzbuzzbuzzbuzzbuzzbz bzbuzzbz bz / bzbuzz buzzbzbuzzbz buzz bzbzbuzz bzbuzz bzbuzzbzbz bzbuzzbzbz buzzbzbuzzbuzz / buzz bzbuzzbz bzbuzz buzzbz bzbzbz bzbuzzbzbz bzbuzz buzz bzbz buzzbz buzzbuzzbz / buzzbuzz buzzbzbuzzbuzz / bzbuzzbuzz buzzbuzzbuzz bzbuzzbz buzzbzbz bzbzbz / buzz bzbzbzbz bz buzzbz / bzbz bzbuzzbuzzbuzzbuzzbz buzzbuzz / bzbz buzzbuzz bzbuzzbuzzbz bzbuzzbz bz bzbzbz bzbzbz bz buzzbzbz</t>
   </si>
   <si>
@@ -340,9 +332,6 @@
     <t>bzbuzz buzzbz buzzbzbz / buzz bzbzbzbz bzbuzz buzz bzbuzzbuzzbuzzbuzzbz bzbzbz / bzbuzz bzbuzzbzbz bzbuzzbzbz bzbuzzbzbuzzbzbuzz / bzbzbz bz bz / buzzbzbuzzbuzz buzzbuzzbuzz bzbzbuzz / bzbuzz bzbuzzbz buzzbuzzbuzz bzbzbuzz buzzbz buzzbzbz</t>
   </si>
   <si>
-    <t>29th</t>
-  </si>
-  <si>
     <t>buzzbzbuzzbuzz bz bzbzbz</t>
   </si>
   <si>
@@ -367,9 +356,6 @@
     <t>Thank you, mysterious grey circle person. I am forever in your debt.</t>
   </si>
   <si>
-    <t>It's not much, but I want you to take this star-sticker I have. Not as a thank you or anything, I was just hoping to get rid of some of my junk.</t>
-  </si>
-  <si>
     <t>Anyway, get off my lawn.</t>
   </si>
   <si>
@@ -421,9 +407,6 @@
     <t>*You decide to make like a flower and run away as far as possible before they can assault your eardrums again.*</t>
   </si>
   <si>
-    <t>2nd</t>
-  </si>
-  <si>
     <t>*It's a really long diatribe. You seriously can't even believe how long a speech this is.*</t>
   </si>
   <si>
@@ -502,18 +485,6 @@
     <t>*You'll never see eye to eye with Darf again, and these flowers clearly don't make for good company. Not to mention the fact that they can't move.*</t>
   </si>
   <si>
-    <t>*You're interrupted in your trance when one of the flowers holds out a leaf holding another, smaller leaf on it, in the shape of a star.*</t>
-  </si>
-  <si>
-    <t>*It seems that they've offered it as thanks for your support. Clearly this was not a mistake after all, and you gladly accept the leafy sticker.*</t>
-  </si>
-  <si>
-    <t>[GOT A STAR STICKER!]</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>*The flowers all murmur in agreement, still transfixed by your original lecture.*</t>
   </si>
   <si>
@@ -538,9 +509,6 @@
     <t>*You see their point and are beginning to doubt if Darf understands gardening very well. But you can probably return to him regardless.*</t>
   </si>
   <si>
-    <t>3rd</t>
-  </si>
-  <si>
     <t>Yes but you'll have to do a few things</t>
   </si>
   <si>
@@ -553,9 +521,6 @@
     <t>flag_values_set</t>
   </si>
   <si>
-    <t>DarfStar</t>
-  </si>
-  <si>
     <t>flags_req</t>
   </si>
   <si>
@@ -572,6 +537,18 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                              </t>
+  </si>
+  <si>
+    <t>*The consequences of this choice will surely have a tremendous effect many generations from now, or at least until you decide to close this game.*</t>
+  </si>
+  <si>
+    <t>FlowerEnd</t>
+  </si>
+  <si>
+    <t>*The flowers are staring at you fondly.*</t>
+  </si>
+  <si>
+    <t>DarfEnd</t>
   </si>
 </sst>
 </file>
@@ -920,8 +897,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1F328B6-531B-46E8-8475-45A00AF286A7}" name="Table1" displayName="Table1" ref="A1:K53" tableType="xml" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:K53" xr:uid="{16DA7A1B-1654-4BAD-91D8-B69F042F6F2B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F1F328B6-531B-46E8-8475-45A00AF286A7}" name="Table1" displayName="Table1" ref="A1:K51" tableType="xml" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:K51" xr:uid="{16DA7A1B-1654-4BAD-91D8-B69F042F6F2B}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{12DDBC33-459E-4D88-A423-04596A58C7CF}" uniqueName="start_id" name="start_id">
       <xmlColumnPr mapId="24" xpath="/graph/edge/@start_id" xmlDataType="integer"/>
@@ -962,8 +939,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8DB0E05-9CF9-4BB1-B306-26E9181D8FDA}" name="Table3" displayName="Table3" ref="A1:K56" tableType="xml" totalsRowShown="0">
-  <autoFilter ref="A1:K56" xr:uid="{14573359-B729-47B4-B28F-336D4F0263CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E8DB0E05-9CF9-4BB1-B306-26E9181D8FDA}" name="Table3" displayName="Table3" ref="A1:K55" tableType="xml" totalsRowShown="0">
+  <autoFilter ref="A1:K55" xr:uid="{14573359-B729-47B4-B28F-336D4F0263CE}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{16BF3D89-49D5-4F84-9053-944910AD2168}" uniqueName="start_id" name="start_id">
       <xmlColumnPr mapId="27" xpath="/graph/edge/@start_id" xmlDataType="integer"/>
@@ -1589,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7427491-4E0D-48E2-B5C6-F016ABF0685E}">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1616,10 +1593,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>12</v>
@@ -1637,10 +1614,10 @@
         <v>11</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1683,9 +1660,6 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1705,12 +1679,6 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="L4">
-        <v>18</v>
-      </c>
-      <c r="M4" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1730,12 +1698,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="L5">
-        <v>28</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1755,12 +1718,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="J6" s="1"/>
-      <c r="L6">
-        <v>27</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>116</v>
-      </c>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1780,12 +1738,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="J7" s="1"/>
-      <c r="L7">
-        <v>46</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>155</v>
-      </c>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1957,7 +1910,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1971,7 +1924,7 @@
         <v>101</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -2002,7 +1955,7 @@
         <v>37</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2022,10 +1975,10 @@
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2041,7 +1994,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -2060,7 +2013,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>20</v>
@@ -2079,7 +2032,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>20</v>
@@ -2098,7 +2051,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>20</v>
@@ -2117,7 +2070,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>20</v>
@@ -2125,7 +2078,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="J24" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K24">
         <v>2</v>
@@ -2139,13 +2092,13 @@
         <v>201</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
@@ -2167,7 +2120,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>20</v>
@@ -2186,10 +2139,10 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2203,16 +2156,16 @@
         <v>300</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2228,15 +2181,15 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="J29" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -2252,7 +2205,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>20</v>
@@ -2271,7 +2224,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>20</v>
@@ -2290,10 +2243,10 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2309,10 +2262,10 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2328,7 +2281,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>20</v>
@@ -2347,10 +2300,10 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2366,10 +2319,10 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2385,10 +2338,10 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2404,10 +2357,10 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2423,7 +2376,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>20</v>
@@ -2431,7 +2384,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="J39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K39">
         <v>3</v>
@@ -2447,7 +2400,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>20</v>
@@ -2466,7 +2419,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>20</v>
@@ -2485,7 +2438,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>20</v>
@@ -2504,7 +2457,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>20</v>
@@ -2521,13 +2474,13 @@
         <v>-1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>20</v>
@@ -2547,13 +2500,13 @@
         <v>501</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>20</v>
@@ -2575,10 +2528,10 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -2592,16 +2545,16 @@
         <v>502</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2617,7 +2570,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>20</v>
@@ -2636,7 +2589,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>20</v>
@@ -2650,90 +2603,67 @@
         <v>504</v>
       </c>
       <c r="B50">
-        <v>505</v>
+        <v>-1</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="J50" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>505</v>
+        <v>0</v>
       </c>
       <c r="B51">
-        <v>506</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
+        <v>-1</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E51" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="J51" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="K51">
-        <v>1</v>
-      </c>
+      <c r="I51">
+        <v>4</v>
+      </c>
+      <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>506</v>
-      </c>
-      <c r="B52">
-        <v>-1</v>
-      </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
-      <c r="J52" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K52">
-        <v>4</v>
-      </c>
+      <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>0</v>
-      </c>
-      <c r="B53">
-        <v>-1</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D53" s="1">
-        <v>4</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53">
-        <v>4</v>
-      </c>
       <c r="J53" s="1"/>
     </row>
   </sheetData>
@@ -2748,8 +2678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719B6289-52A4-476D-9CF1-BA5030BC834B}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,10 +2704,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>12</v>
@@ -2795,10 +2725,10 @@
         <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="K1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2811,7 +2741,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -2829,13 +2759,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -2855,10 +2785,10 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -2874,10 +2804,10 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -2893,10 +2823,10 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -2912,10 +2842,10 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -2931,10 +2861,10 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -2950,10 +2880,10 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -2969,7 +2899,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -2986,7 +2916,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3003,7 +2933,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -3020,7 +2950,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -3037,7 +2967,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -3054,7 +2984,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -3071,7 +3001,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -3088,7 +3018,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -3105,7 +3035,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -3125,17 +3055,15 @@
         <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>164</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19">
@@ -3153,10 +3081,10 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -3172,10 +3100,10 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -3191,9 +3119,11 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>153</v>
+      </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="J22" s="1"/>
@@ -3208,7 +3138,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
@@ -3225,7 +3155,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -3242,7 +3172,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -3259,7 +3189,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -3276,7 +3206,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -3293,7 +3223,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
@@ -3310,10 +3240,10 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -3329,10 +3259,10 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -3348,10 +3278,10 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -3367,10 +3297,10 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -3386,7 +3316,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -3403,7 +3333,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -3420,7 +3350,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
@@ -3437,7 +3367,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -3454,7 +3384,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -3471,7 +3401,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -3488,7 +3418,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -3505,7 +3435,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -3522,7 +3452,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -3539,7 +3469,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -3556,7 +3486,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -3573,7 +3503,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -3590,13 +3520,13 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="J45" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -3610,11 +3540,11 @@
         <v>401</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -3624,7 +3554,7 @@
       </c>
       <c r="J46" s="1"/>
       <c r="K46" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -3637,7 +3567,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -3654,14 +3584,14 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>403</v>
       </c>
@@ -3671,14 +3601,14 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>404</v>
       </c>
@@ -3688,14 +3618,14 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>405</v>
       </c>
@@ -3705,14 +3635,14 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>406</v>
       </c>
@@ -3722,14 +3652,14 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>407</v>
       </c>
@@ -3739,59 +3669,63 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>408</v>
       </c>
       <c r="B54">
-        <v>409</v>
+        <v>-1</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
-      <c r="J54" s="1"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>409</v>
+        <v>0</v>
       </c>
       <c r="B55">
-        <v>410</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
+        <v>-1</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="E55" s="1" t="s">
-        <v>144</v>
+        <v>158</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
+      <c r="I55">
+        <v>4</v>
+      </c>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>410</v>
-      </c>
-      <c r="B56">
-        <v>-1</v>
-      </c>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>145</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -3836,10 +3770,10 @@
         <v>10</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>12</v>
@@ -3857,10 +3791,10 @@
         <v>11</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -3873,10 +3807,10 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3892,10 +3826,10 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3911,10 +3845,10 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3930,10 +3864,10 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -3947,16 +3881,16 @@
         <v>200</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -3972,10 +3906,10 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -3991,10 +3925,10 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -4010,10 +3944,10 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -4029,10 +3963,10 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -4048,10 +3982,10 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -4067,10 +4001,10 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -4086,10 +4020,10 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -4105,10 +4039,10 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -4124,10 +4058,10 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -4143,10 +4077,10 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -4162,10 +4096,10 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -4181,10 +4115,10 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -4200,10 +4134,10 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -4219,10 +4153,10 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -4238,10 +4172,10 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -4257,10 +4191,10 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -4276,10 +4210,10 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -4295,10 +4229,10 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -4314,15 +4248,15 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="J25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -4334,74 +4268,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD042D1-A493-4399-9FE3-B910DBECE0BE}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="131.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711BD744-84E5-42BC-8821-05514EFD4421}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>